<commit_message>
- added Visio documents - added mind maps - changed Schätzsheet
</commit_message>
<xml_diff>
--- a/02_Projektleitung/01_Planung/01_Gesamtprojektplan/Schätzsheet.xlsx
+++ b/02_Projektleitung/01_Planung/01_Gesamtprojektplan/Schätzsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Eclipse Plug-in Env</t>
   </si>
@@ -169,13 +169,16 @@
   </si>
   <si>
     <t>/22h/w =&gt; #w</t>
+  </si>
+  <si>
+    <t>done?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +194,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +239,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -251,17 +272,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -277,6 +296,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,14 +315,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -589,125 +613,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:15">
+      <c r="E1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="21"/>
+      <c r="N1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6">
-        <v>4</v>
-      </c>
-      <c r="F3" s="7">
-        <v>2</v>
+      <c r="C3" s="17">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
       </c>
       <c r="G3" s="6">
-        <v>4</v>
-      </c>
-      <c r="H3" s="16">
-        <v>4</v>
-      </c>
-      <c r="I3" s="16">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4</v>
+      </c>
+      <c r="I3" s="11">
+        <v>4</v>
+      </c>
+      <c r="J3" s="11">
         <v>8</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="18">
-        <f>AVERAGE(D3,F3,H3)</f>
+      <c r="K3" s="1"/>
+      <c r="L3" s="13">
+        <f>AVERAGE(E3,G3,I3)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="L3" s="18">
-        <f>AVERAGE(E3,G3,I3)</f>
+      <c r="M3" s="13">
+        <f>AVERAGE(F3,H3,J3)</f>
         <v>5.333333333333333</v>
       </c>
-      <c r="M3" s="18">
-        <f>C3*K3</f>
+      <c r="N3" s="13">
+        <f>D3*L3</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="N3" s="18">
-        <f>C3*L3</f>
+      <c r="O3" s="13">
+        <f>D3*M3</f>
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -715,45 +746,48 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="7">
-        <v>3</v>
-      </c>
       <c r="G4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5">
         <v>6</v>
       </c>
-      <c r="H4" s="16">
-        <v>3</v>
-      </c>
-      <c r="I4" s="16">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="18">
-        <f t="shared" ref="K4:L19" si="0">AVERAGE(D4,F4,H4)</f>
+      <c r="I4" s="11">
+        <v>3</v>
+      </c>
+      <c r="J4" s="11">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="13">
+        <f t="shared" ref="L4:M19" si="0">AVERAGE(E4,G4,I4)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="L4" s="18">
+      <c r="M4" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M4" s="18">
-        <f t="shared" ref="M4:M19" si="1">C4*K4</f>
+      <c r="N4" s="13">
+        <f t="shared" ref="N4:N19" si="1">D4*L4</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="N4" s="18">
-        <f t="shared" ref="N4:N19" si="2">C4*L4</f>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O19" si="2">D4*M4</f>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -761,41 +795,44 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
         <v>5</v>
       </c>
-      <c r="F5" s="7">
-        <v>3</v>
-      </c>
       <c r="G5" s="6">
-        <v>4</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L5" s="18">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M5" s="13">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="M5" s="18">
+      <c r="N5" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N5" s="18">
+      <c r="O5" s="13">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -803,45 +840,48 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="16">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5">
         <v>8</v>
       </c>
-      <c r="F6" s="7">
-        <v>3</v>
-      </c>
       <c r="G6" s="6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
         <v>6</v>
       </c>
-      <c r="H6" s="16">
-        <v>4</v>
-      </c>
-      <c r="I6" s="16">
+      <c r="I6" s="11">
+        <v>4</v>
+      </c>
+      <c r="J6" s="11">
         <v>7</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="18">
+      <c r="K6" s="1"/>
+      <c r="L6" s="13">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="L6" s="18">
+      <c r="M6" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="M6" s="18">
+      <c r="N6" s="13">
         <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="N6" s="18">
+      <c r="O6" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -849,39 +889,42 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="16">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>3</v>
-      </c>
-      <c r="F7" s="7">
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5">
         <v>3</v>
       </c>
       <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="5">
         <v>5</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="18">
+      <c r="K7" s="1"/>
+      <c r="L7" s="13">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="L7" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M7" s="18">
+      <c r="M7" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="13">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N7" s="18">
+      <c r="O7" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -889,39 +932,42 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="6">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
       </c>
       <c r="G8" s="6">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="18">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="13">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="L8" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="M8" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N8" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N8" s="18">
+      <c r="O8" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -929,39 +975,42 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>4</v>
-      </c>
-      <c r="F9" s="7">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
       </c>
       <c r="G9" s="6">
-        <v>4</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M9" s="18">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N9" s="13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="N9" s="18">
+      <c r="O9" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -969,79 +1018,82 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="6">
-        <v>4</v>
-      </c>
-      <c r="F10" s="7">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4</v>
       </c>
       <c r="G10" s="6">
-        <v>3</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="18">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="13">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="L10" s="18">
+      <c r="M10" s="13">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="M10" s="18">
+      <c r="N10" s="13">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="N10" s="18">
+      <c r="O10" s="13">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16">
-        <v>3</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5">
         <v>6</v>
       </c>
-      <c r="F11" s="7">
-        <v>3</v>
-      </c>
       <c r="G11" s="6">
+        <v>3</v>
+      </c>
+      <c r="H11" s="5">
         <v>5</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L11" s="18">
+      <c r="K11" s="2"/>
+      <c r="L11" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M11" s="13">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="M11" s="18">
+      <c r="N11" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N11" s="18">
+      <c r="O11" s="13">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1049,491 +1101,494 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="16">
-        <v>4</v>
-      </c>
-      <c r="E12" s="6">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5">
         <v>8</v>
       </c>
-      <c r="F12" s="7">
-        <v>2</v>
-      </c>
       <c r="G12" s="6">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5">
         <v>6</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L12" s="18">
+      <c r="K12" s="2"/>
+      <c r="L12" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M12" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="M12" s="18">
+      <c r="N12" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N12" s="18">
+      <c r="O12" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1.5</v>
       </c>
-      <c r="D13" s="16">
-        <v>3</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="E13" s="11">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
         <v>5</v>
       </c>
-      <c r="F13" s="7">
-        <v>2</v>
-      </c>
       <c r="G13" s="6">
-        <v>4</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="18">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="13">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="L13" s="18">
+      <c r="M13" s="13">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="M13" s="18">
+      <c r="N13" s="13">
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
-      <c r="N13" s="18">
+      <c r="O13" s="13">
         <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="16">
-        <v>4</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <v>4</v>
+      </c>
+      <c r="F14" s="5">
         <v>8</v>
       </c>
-      <c r="F14" s="7">
-        <v>3</v>
-      </c>
       <c r="G14" s="6">
+        <v>3</v>
+      </c>
+      <c r="H14" s="5">
         <v>6</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="18">
+      <c r="K14" s="2"/>
+      <c r="L14" s="13">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="L14" s="18">
+      <c r="M14" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="M14" s="18">
+      <c r="N14" s="13">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="N14" s="18">
+      <c r="O14" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
         <v>1</v>
       </c>
       <c r="G15" s="6">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="18">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="13">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="M15" s="18">
+      <c r="N15" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N15" s="18">
+      <c r="O15" s="13">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5">
         <v>5</v>
       </c>
-      <c r="F16" s="7">
-        <v>3</v>
-      </c>
       <c r="G16" s="6">
+        <v>3</v>
+      </c>
+      <c r="H16" s="5">
         <v>6</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L16" s="18">
+      <c r="K16" s="2"/>
+      <c r="L16" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M16" s="13">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="M16" s="18">
+      <c r="N16" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N16" s="18">
+      <c r="O16" s="13">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="16">
-        <v>4</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
         <v>10</v>
       </c>
-      <c r="F17" s="7">
-        <v>2</v>
-      </c>
       <c r="G17" s="6">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5">
         <v>8</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L17" s="18">
+      <c r="K17" s="2"/>
+      <c r="L17" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M17" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M17" s="18">
+      <c r="N17" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N17" s="18">
+      <c r="O17" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
+    <row r="18" spans="1:15">
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="6"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="H18" s="5"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
         <v>6</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="5">
         <v>8</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="6">
         <v>5</v>
       </c>
-      <c r="G19" s="6">
+      <c r="H19" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="18">
+      <c r="L19" s="13">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="L19" s="18">
+      <c r="M19" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M19" s="18">
+      <c r="N19" s="13">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="N19" s="18">
+      <c r="O19" s="13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
+    <row r="20" spans="1:15">
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="6"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="H20" s="5"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="6"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="H21" s="5"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="6"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="H22" s="5"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="6"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="H23" s="5"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="6"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="H24" s="5"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="6"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="6"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="H26" s="5"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="6"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="H27" s="5"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="K30" s="18"/>
-      <c r="L30" t="s">
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="L30" s="13"/>
+      <c r="M30" t="s">
         <v>38</v>
       </c>
-      <c r="M30" s="18">
-        <f>SUM(M3:M10)</f>
+      <c r="N30" s="13">
+        <f>SUM(N3:N10)</f>
         <v>24.833333333333336</v>
       </c>
-      <c r="N30" s="18">
-        <f>SUM(N3:N10)</f>
+      <c r="O30" s="13">
+        <f>SUM(O3:O10)</f>
         <v>42.333333333333329</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
-      <c r="K31" s="18"/>
-      <c r="L31" t="s">
+    <row r="31" spans="1:15">
+      <c r="L31" s="13"/>
+      <c r="M31" t="s">
         <v>39</v>
       </c>
-      <c r="M31" s="18">
-        <f>M30/8</f>
+      <c r="N31" s="13">
+        <f>N30/8</f>
         <v>3.104166666666667</v>
       </c>
-      <c r="N31" s="18">
-        <f>N30/8</f>
+      <c r="O31" s="13">
+        <f>O30/8</f>
         <v>5.2916666666666661</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
-      <c r="L32" s="20" t="s">
+    <row r="32" spans="1:15">
+      <c r="M32" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="M32">
-        <f>M30/22</f>
-        <v>1.1287878787878789</v>
       </c>
       <c r="N32">
         <f>N30/22</f>
+        <v>1.1287878787878789</v>
+      </c>
+      <c r="O32">
+        <f>O30/22</f>
         <v>1.9242424242424241</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="M33" s="21">
-        <f ca="1">TODAY()+M32*7</f>
-        <v>39779.901515151512</v>
-      </c>
-      <c r="N33" s="21">
+      <c r="N33" s="16">
         <f ca="1">TODAY()+N32*7</f>
-        <v>39785.469696969696</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>39797.901515151512</v>
+      </c>
+      <c r="O33" s="16">
+        <f ca="1">TODAY()+O32*7</f>
+        <v>39803.469696969696</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1541,7 +1596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1604,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1557,7 +1612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1565,7 +1620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1575,12 +1630,24 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C1048576 C1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>